<commit_message>
Few changes date format in reports and excel export
</commit_message>
<xml_diff>
--- a/public/assets/MonthlyReportSample3test.xlsx
+++ b/public/assets/MonthlyReportSample3test.xlsx
@@ -353,8 +353,8 @@
   </sheetPr>
   <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T9" activeCellId="1" sqref="R:R T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -362,7 +362,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +481,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>39</v>
       </c>

</xml_diff>